<commit_message>
ugly regex in place of ct
</commit_message>
<xml_diff>
--- a/rules/NEW-RULE/negative/01/data/new-rule-negative-01.xlsx
+++ b/rules/NEW-RULE/negative/01/data/new-rule-negative-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/github/core-contributor/rules/NEW-RULE/negative/01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9676CB03-F50D-D244-A170-F854FAA6D4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3FED30-5F76-FF48-B11E-C147E619727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
   <si>
     <t>Product</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Record</t>
+  </si>
+  <si>
+    <t>Associated Persons Laboratory Test Results</t>
   </si>
 </sst>
 </file>
@@ -631,9 +634,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -643,6 +648,14 @@
       </c>
       <c r="B1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjust negative test case
</commit_message>
<xml_diff>
--- a/rules/NEW-RULE/negative/01/data/new-rule-negative-01.xlsx
+++ b/rules/NEW-RULE/negative/01/data/new-rule-negative-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/github/core-contributor/rules/NEW-RULE/negative/01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61A4AA-1D77-D642-B13A-89EC4D07774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC51CF8-0DA8-D541-A3FF-7AFB97C5E728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Product</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Record</t>
-  </si>
-  <si>
-    <t>pmol/L/ug</t>
   </si>
   <si>
     <t>day*ug/mL/mg</t>
@@ -799,7 +796,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1031,7 @@
         <v>1194.546</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" s="7">
         <v>1195</v>

</xml_diff>